<commit_message>
adding result of RMAT25
</commit_message>
<xml_diff>
--- a/Results/Results/result analysis_final.xlsx
+++ b/Results/Results/result analysis_final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="RMAT24" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="hollywood-2009" sheetId="5" r:id="rId5"/>
     <sheet name="roadNet-CA" sheetId="6" r:id="rId6"/>
     <sheet name="soc-orkut" sheetId="7" r:id="rId7"/>
+    <sheet name="RMAT25.graph500" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="29">
   <si>
     <t>Graph name:</t>
   </si>
@@ -114,6 +115,9 @@
   </si>
   <si>
     <t>SSSP update Async(in millisec)</t>
+  </si>
+  <si>
+    <t>RMAT25.graph50</t>
   </si>
 </sst>
 </file>
@@ -243,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -259,17 +263,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,18 +594,18 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16" t="s">
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="21" t="s">
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -629,10 +634,10 @@
       <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -652,14 +657,14 @@
       <c r="I7" s="6">
         <v>255.791</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <f>H7+I7</f>
         <v>496.363</v>
       </c>
       <c r="L7" s="11">
         <v>1988.4920119999999</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="16">
         <v>583.33000000000004</v>
       </c>
     </row>
@@ -679,14 +684,14 @@
       <c r="I8" s="6">
         <v>164.47200000000001</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="16">
         <f t="shared" ref="J8:J26" si="0">H8+I8</f>
         <v>705.70699999999999</v>
       </c>
       <c r="L8" s="6">
         <v>1932.6429370000001</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="16">
         <v>746.80600000000004</v>
       </c>
     </row>
@@ -706,14 +711,14 @@
       <c r="I9" s="6">
         <v>217.97399999999999</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="16">
         <f t="shared" si="0"/>
         <v>757.37200000000007</v>
       </c>
       <c r="L9" s="6">
         <v>1914.3331049999999</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="16">
         <v>750.01800000000003</v>
       </c>
     </row>
@@ -733,14 +738,14 @@
       <c r="I10" s="6">
         <v>315.536</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="16">
         <f t="shared" si="0"/>
         <v>863.15100000000007</v>
       </c>
       <c r="L10" s="6">
         <v>1902.544022</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="16">
         <v>802.98</v>
       </c>
     </row>
@@ -760,14 +765,14 @@
       <c r="I11" s="6">
         <v>315.74099999999999</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="16">
         <f t="shared" si="0"/>
         <v>840.95299999999997</v>
       </c>
       <c r="L11" s="6">
         <v>1911.00812</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="16">
         <v>801.827</v>
       </c>
     </row>
@@ -787,14 +792,14 @@
       <c r="I12" s="6">
         <v>292.36700000000002</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="16">
         <f t="shared" si="0"/>
         <v>543.53300000000002</v>
       </c>
       <c r="L12" s="11">
         <v>1962.653875</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="16">
         <v>617.89300000000003</v>
       </c>
     </row>
@@ -814,14 +819,14 @@
       <c r="I13" s="6">
         <v>377.166</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="16">
         <f t="shared" si="0"/>
         <v>953.65300000000002</v>
       </c>
       <c r="L13" s="11">
         <v>1971.4589120000001</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="16">
         <v>855.12199999999996</v>
       </c>
     </row>
@@ -841,14 +846,14 @@
       <c r="I14" s="6">
         <v>545.21199999999999</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="16">
         <f t="shared" si="0"/>
         <v>1123.675</v>
       </c>
       <c r="L14" s="11">
         <v>1929.384947</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="16">
         <v>987.65</v>
       </c>
     </row>
@@ -868,14 +873,14 @@
       <c r="I15" s="6">
         <v>679.75699999999995</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="16">
         <f t="shared" si="0"/>
         <v>1266.674</v>
       </c>
       <c r="L15" s="11">
         <v>1997.2069260000001</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="16">
         <v>1132.45</v>
       </c>
     </row>
@@ -895,14 +900,14 @@
       <c r="I16" s="6">
         <v>916.73500000000001</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="16">
         <f t="shared" si="0"/>
         <v>1522.346</v>
       </c>
       <c r="L16" s="11">
         <v>1936.9108679999999</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="16">
         <v>1226.06</v>
       </c>
     </row>
@@ -922,14 +927,14 @@
       <c r="I17" s="6">
         <v>318.7</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="16">
         <f t="shared" si="0"/>
         <v>590.46100000000001</v>
       </c>
       <c r="L17" s="11">
         <v>2112.9531860000002</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="16">
         <v>659.42700000000002</v>
       </c>
     </row>
@@ -949,14 +954,14 @@
       <c r="I18" s="6">
         <v>587.48400000000004</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="16">
         <f t="shared" si="0"/>
         <v>1197.0350000000001</v>
       </c>
       <c r="L18" s="11">
         <v>1997.0278740000001</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="16">
         <v>1079.3499999999999</v>
       </c>
     </row>
@@ -976,14 +981,14 @@
       <c r="I19" s="6">
         <v>952.36400000000003</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="16">
         <f t="shared" si="0"/>
         <v>1574.643</v>
       </c>
       <c r="L19" s="11">
         <v>1962.9662040000001</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="16">
         <v>1447.23</v>
       </c>
     </row>
@@ -1010,7 +1015,7 @@
       <c r="L20" s="11">
         <v>1954.1418550000001</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="16">
         <v>1617.71</v>
       </c>
     </row>
@@ -1037,7 +1042,7 @@
       <c r="L21" s="11">
         <v>1900.4900459999999</v>
       </c>
-      <c r="N21" s="18">
+      <c r="N21" s="16">
         <v>1735.44</v>
       </c>
     </row>
@@ -1057,14 +1062,14 @@
       <c r="I22" s="6">
         <v>445.935</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="16">
         <f t="shared" si="0"/>
         <v>718.81400000000008</v>
       </c>
       <c r="L22" s="11">
         <v>2416.2631029999998</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="16">
         <v>823.69100000000003</v>
       </c>
     </row>
@@ -1091,7 +1096,7 @@
       <c r="L23" s="11">
         <v>2371.4489939999999</v>
       </c>
-      <c r="N23" s="18">
+      <c r="N23" s="16">
         <v>2283.23</v>
       </c>
     </row>
@@ -1226,17 +1231,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -1283,7 +1288,7 @@
       <c r="H7" s="6">
         <v>36.927999999999997</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="15">
         <f>G7+H7</f>
         <v>85.771000000000001</v>
       </c>
@@ -1307,7 +1312,7 @@
       <c r="H8" s="6">
         <v>125.232</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="15">
         <f t="shared" ref="I8:I21" si="0">G8+H8</f>
         <v>262.80099999999999</v>
       </c>
@@ -1331,7 +1336,7 @@
       <c r="H9" s="6">
         <v>116.739</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="15">
         <f t="shared" si="0"/>
         <v>271.245</v>
       </c>
@@ -1355,7 +1360,7 @@
       <c r="H10" s="6">
         <v>123.438</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="15">
         <f t="shared" si="0"/>
         <v>305.90600000000001</v>
       </c>
@@ -1379,7 +1384,7 @@
       <c r="H11" s="6">
         <v>107.649</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="15">
         <f t="shared" si="0"/>
         <v>291.16200000000003</v>
       </c>
@@ -1403,7 +1408,7 @@
       <c r="H12" s="6">
         <v>49.027999999999999</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="15">
         <f t="shared" si="0"/>
         <v>108.715</v>
       </c>
@@ -1427,7 +1432,7 @@
       <c r="H13" s="6">
         <v>83.757000000000005</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="15">
         <f t="shared" si="0"/>
         <v>341.685</v>
       </c>
@@ -1523,7 +1528,7 @@
       <c r="H17" s="6">
         <v>127.657</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="16">
         <f t="shared" si="0"/>
         <v>248.19299999999998</v>
       </c>
@@ -1682,17 +1687,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -1958,17 +1963,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -2015,7 +2020,7 @@
       <c r="H7" s="6">
         <v>55.731000000000002</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <f>G7+H7</f>
         <v>109.721</v>
       </c>
@@ -2039,7 +2044,7 @@
       <c r="H8" s="6">
         <v>45.005000000000003</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <f t="shared" ref="I8:I21" si="0">G8+H8</f>
         <v>177.91200000000001</v>
       </c>
@@ -2063,7 +2068,7 @@
       <c r="H9" s="6">
         <v>49.712000000000003</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
         <v>208.32499999999999</v>
       </c>
@@ -2087,7 +2092,7 @@
       <c r="H10" s="6">
         <v>50.183</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
         <v>233.274</v>
       </c>
@@ -2111,7 +2116,7 @@
       <c r="H11" s="6">
         <v>48.177</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <f t="shared" si="0"/>
         <v>227.28100000000001</v>
       </c>
@@ -2135,7 +2140,7 @@
       <c r="H12" s="6">
         <v>70.150000000000006</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="16">
         <f t="shared" si="0"/>
         <v>145.626</v>
       </c>
@@ -2159,7 +2164,7 @@
       <c r="H13" s="6">
         <v>49.701000000000001</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="16">
         <f t="shared" si="0"/>
         <v>289.38499999999999</v>
       </c>
@@ -2255,7 +2260,7 @@
       <c r="H17" s="6">
         <v>77.88</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="16">
         <f t="shared" si="0"/>
         <v>217.761</v>
       </c>
@@ -2412,17 +2417,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -2469,7 +2474,7 @@
       <c r="H7" s="6">
         <v>33.914000000000001</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <f>G7+H7</f>
         <v>82.490000000000009</v>
       </c>
@@ -2493,7 +2498,7 @@
       <c r="H8" s="6">
         <v>25.649000000000001</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <f t="shared" ref="I8:I21" si="0">G8+H8</f>
         <v>126.277</v>
       </c>
@@ -2517,7 +2522,7 @@
       <c r="H9" s="6">
         <v>26.713999999999999</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
         <v>138.19999999999999</v>
       </c>
@@ -2541,7 +2546,7 @@
       <c r="H10" s="6">
         <v>24.062999999999999</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
         <v>139.166</v>
       </c>
@@ -2565,7 +2570,7 @@
       <c r="H11" s="6">
         <v>27.265000000000001</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <f t="shared" si="0"/>
         <v>151.92099999999999</v>
       </c>
@@ -2589,7 +2594,7 @@
       <c r="H12" s="6">
         <v>92.009</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="16">
         <f t="shared" si="0"/>
         <v>188.66399999999999</v>
       </c>
@@ -2613,7 +2618,7 @@
       <c r="H13" s="6">
         <v>36.161999999999999</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="16">
         <f t="shared" si="0"/>
         <v>190.21899999999999</v>
       </c>
@@ -2637,7 +2642,7 @@
       <c r="H14" s="6">
         <v>76.534000000000006</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="16">
         <f t="shared" si="0"/>
         <v>268.22199999999998</v>
       </c>
@@ -2661,7 +2666,7 @@
       <c r="H15" s="6">
         <v>49.676000000000002</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="16">
         <f t="shared" si="0"/>
         <v>287.23099999999999</v>
       </c>
@@ -2685,7 +2690,7 @@
       <c r="H16" s="6">
         <v>44.106999999999999</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="16">
         <f t="shared" si="0"/>
         <v>314.94100000000003</v>
       </c>
@@ -2709,7 +2714,7 @@
       <c r="H17" s="6">
         <v>89.116</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="16">
         <f t="shared" si="0"/>
         <v>163.41800000000001</v>
       </c>
@@ -2733,7 +2738,7 @@
       <c r="H18" s="6">
         <v>70.031000000000006</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="16">
         <f t="shared" si="0"/>
         <v>283.02800000000002</v>
       </c>
@@ -2882,17 +2887,17 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -3137,17 +3142,17 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -3194,7 +3199,7 @@
       <c r="H6" s="6">
         <v>130.29</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <f>G6+H6</f>
         <v>235.07599999999999</v>
       </c>
@@ -3218,7 +3223,7 @@
       <c r="H7" s="6">
         <v>53.125999999999998</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <f t="shared" ref="I7:I25" si="0">G7+H7</f>
         <v>301.26099999999997</v>
       </c>
@@ -3242,7 +3247,7 @@
       <c r="H8" s="6">
         <v>52.41</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <f t="shared" si="0"/>
         <v>307.63900000000001</v>
       </c>
@@ -3266,7 +3271,7 @@
       <c r="H9" s="6">
         <v>50.298000000000002</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
         <v>311.00600000000003</v>
       </c>
@@ -3290,7 +3295,7 @@
       <c r="H10" s="6">
         <v>46.723999999999997</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
         <v>311.077</v>
       </c>
@@ -3314,7 +3319,7 @@
       <c r="H11" s="6">
         <v>170.75299999999999</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <f t="shared" si="0"/>
         <v>331.48899999999998</v>
       </c>
@@ -3338,7 +3343,7 @@
       <c r="H12" s="6">
         <v>76.287999999999997</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="16">
         <f t="shared" si="0"/>
         <v>372.46300000000002</v>
       </c>
@@ -3362,7 +3367,7 @@
       <c r="H13" s="6">
         <v>66.245000000000005</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="16">
         <f t="shared" si="0"/>
         <v>396.13200000000001</v>
       </c>
@@ -3386,7 +3391,7 @@
       <c r="H14" s="6">
         <v>70.03</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="16">
         <f t="shared" si="0"/>
         <v>437.83000000000004</v>
       </c>
@@ -3410,7 +3415,7 @@
       <c r="H15" s="6">
         <v>76.864999999999995</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="16">
         <f t="shared" si="0"/>
         <v>464.84500000000003</v>
       </c>
@@ -3434,7 +3439,7 @@
       <c r="H16" s="6">
         <v>171.99700000000001</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="16">
         <f t="shared" si="0"/>
         <v>299.72500000000002</v>
       </c>
@@ -3458,7 +3463,7 @@
       <c r="H17" s="6">
         <v>82.509</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="16">
         <f t="shared" si="0"/>
         <v>436.90600000000001</v>
       </c>
@@ -3482,7 +3487,7 @@
       <c r="H18" s="6">
         <v>88.962999999999994</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="16">
         <f t="shared" si="0"/>
         <v>517.62400000000002</v>
       </c>
@@ -3506,7 +3511,7 @@
       <c r="H19" s="6">
         <v>88.391999999999996</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="16">
         <f t="shared" si="0"/>
         <v>579.928</v>
       </c>
@@ -3530,7 +3535,7 @@
       <c r="H20" s="6">
         <v>94.947999999999993</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="16">
         <f t="shared" si="0"/>
         <v>623.73299999999995</v>
       </c>
@@ -3554,7 +3559,7 @@
       <c r="H21" s="6">
         <v>273.99599999999998</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="16">
         <f t="shared" si="0"/>
         <v>505.25799999999998</v>
       </c>
@@ -3656,6 +3661,578 @@
       </c>
       <c r="K25" s="11">
         <v>525.43091800000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>33554431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>287295061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>2321.6</v>
+      </c>
+      <c r="G6">
+        <v>271.678</v>
+      </c>
+      <c r="H6">
+        <v>270.96600000000001</v>
+      </c>
+      <c r="I6" s="22">
+        <f>G6+H6</f>
+        <v>542.64400000000001</v>
+      </c>
+      <c r="K6">
+        <v>2406.0418610000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1">
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <v>2317.02</v>
+      </c>
+      <c r="G7">
+        <v>872.65499999999997</v>
+      </c>
+      <c r="H7">
+        <v>558.84100000000001</v>
+      </c>
+      <c r="I7" s="22">
+        <f t="shared" ref="I7:I25" si="0">G7+H7</f>
+        <v>1431.4960000000001</v>
+      </c>
+      <c r="K7">
+        <v>3407.979965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>2312.0300000000002</v>
+      </c>
+      <c r="G8">
+        <v>1052.19</v>
+      </c>
+      <c r="H8">
+        <v>585.06700000000001</v>
+      </c>
+      <c r="I8" s="22">
+        <f t="shared" si="0"/>
+        <v>1637.2570000000001</v>
+      </c>
+      <c r="K8">
+        <v>2316.7428970000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>2308.1799999999998</v>
+      </c>
+      <c r="G9">
+        <v>1168.17</v>
+      </c>
+      <c r="H9">
+        <v>592.27700000000004</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="0"/>
+        <v>1760.4470000000001</v>
+      </c>
+      <c r="K9">
+        <v>2303.6310669999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2308.86</v>
+      </c>
+      <c r="G10">
+        <v>1291</v>
+      </c>
+      <c r="H10">
+        <v>598.25199999999995</v>
+      </c>
+      <c r="I10" s="22">
+        <f t="shared" si="0"/>
+        <v>1889.252</v>
+      </c>
+      <c r="K10">
+        <v>2296.5309619999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>2420.59</v>
+      </c>
+      <c r="G11">
+        <v>286.38400000000001</v>
+      </c>
+      <c r="H11">
+        <v>656.33600000000001</v>
+      </c>
+      <c r="I11" s="22">
+        <f t="shared" si="0"/>
+        <v>942.72</v>
+      </c>
+      <c r="K11">
+        <v>2321.5749259999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1">
+        <v>75</v>
+      </c>
+      <c r="F12">
+        <v>2395.7800000000002</v>
+      </c>
+      <c r="G12">
+        <v>1596.12</v>
+      </c>
+      <c r="H12">
+        <v>970.13099999999997</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>2566.2509999999997</v>
+      </c>
+      <c r="K12">
+        <v>2311.5830420000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>2377.7399999999998</v>
+      </c>
+      <c r="G13">
+        <v>2419.61</v>
+      </c>
+      <c r="H13">
+        <v>568.81299999999999</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>2988.4230000000002</v>
+      </c>
+      <c r="K13">
+        <v>2328.7220000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1">
+        <v>25</v>
+      </c>
+      <c r="F14">
+        <v>2394.9499999999998</v>
+      </c>
+      <c r="G14">
+        <v>3041.1</v>
+      </c>
+      <c r="H14">
+        <v>728.29</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>3769.39</v>
+      </c>
+      <c r="K14">
+        <v>2314.6948809999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2376.39</v>
+      </c>
+      <c r="G15">
+        <v>3703.63</v>
+      </c>
+      <c r="H15">
+        <v>2023.88</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>5727.51</v>
+      </c>
+      <c r="K15">
+        <v>2304.7230239999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="7">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>2625.45</v>
+      </c>
+      <c r="G16">
+        <v>304.005</v>
+      </c>
+      <c r="H16">
+        <v>666.274</v>
+      </c>
+      <c r="I16" s="22">
+        <f t="shared" si="0"/>
+        <v>970.279</v>
+      </c>
+      <c r="K16">
+        <v>2365.3590680000002</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>2483.54</v>
+      </c>
+      <c r="G17">
+        <v>2463.4299999999998</v>
+      </c>
+      <c r="H17">
+        <v>925.55200000000002</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>3388.982</v>
+      </c>
+      <c r="K17">
+        <v>2329.5168880000001</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1">
+        <v>50</v>
+      </c>
+      <c r="F18">
+        <v>2482.44</v>
+      </c>
+      <c r="G18">
+        <v>4188.17</v>
+      </c>
+      <c r="H18">
+        <v>1995.57</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>6183.74</v>
+      </c>
+      <c r="K18">
+        <v>2302.1829130000001</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1">
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <v>2449.66</v>
+      </c>
+      <c r="G19">
+        <v>5427.75</v>
+      </c>
+      <c r="H19">
+        <v>5088.0200000000004</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>10515.77</v>
+      </c>
+      <c r="K19">
+        <v>2289.4999979999998</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2414.36</v>
+      </c>
+      <c r="G20">
+        <v>6657.16</v>
+      </c>
+      <c r="H20">
+        <v>6632.47</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>13289.630000000001</v>
+      </c>
+      <c r="K20">
+        <v>2388.4980679999999</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="7">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>3483.82</v>
+      </c>
+      <c r="G21">
+        <v>424.49</v>
+      </c>
+      <c r="H21">
+        <v>866.28</v>
+      </c>
+      <c r="I21" s="22">
+        <f t="shared" si="0"/>
+        <v>1290.77</v>
+      </c>
+      <c r="K21">
+        <v>2522.5131510000001</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1">
+        <v>75</v>
+      </c>
+      <c r="F22">
+        <v>3256.99</v>
+      </c>
+      <c r="G22">
+        <v>9476.9599999999991</v>
+      </c>
+      <c r="H22">
+        <v>1232.17</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>10709.13</v>
+      </c>
+      <c r="K22">
+        <v>2421.3621619999999</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>3063.4</v>
+      </c>
+      <c r="G23">
+        <v>18291.5</v>
+      </c>
+      <c r="H23">
+        <v>1576.74</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>19868.240000000002</v>
+      </c>
+      <c r="K23">
+        <v>2306.1168189999999</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <v>3001.59</v>
+      </c>
+      <c r="G24">
+        <v>24155.5</v>
+      </c>
+      <c r="H24">
+        <v>1939.82</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>26095.32</v>
+      </c>
+      <c r="K24">
+        <v>2250.5960460000001</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2873.7</v>
+      </c>
+      <c r="G25">
+        <v>30391.7</v>
+      </c>
+      <c r="H25">
+        <v>6361.17</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>36752.870000000003</v>
+      </c>
+      <c r="K25">
+        <v>2131.5040589999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding 25M change result
</commit_message>
<xml_diff>
--- a/Results/Results/result analysis_final.xlsx
+++ b/Results/Results/result analysis_final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RMAT24" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="30">
   <si>
     <t>Graph name:</t>
   </si>
@@ -119,6 +119,9 @@
   <si>
     <t>RMAT25.graph50</t>
   </si>
+  <si>
+    <t>25M</t>
+  </si>
 </sst>
 </file>
 
@@ -183,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -243,11 +246,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -268,13 +282,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,17 +609,17 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21" t="s">
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
       <c r="N5" s="19" t="s">
         <v>27</v>
       </c>
@@ -685,7 +700,7 @@
         <v>164.47200000000001</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" ref="J8:J26" si="0">H8+I8</f>
+        <f t="shared" ref="J8:J31" si="0">H8+I8</f>
         <v>705.70699999999999</v>
       </c>
       <c r="L8" s="6">
@@ -1179,6 +1194,111 @@
       </c>
       <c r="N26" s="2">
         <v>2589.66</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="7">
+        <v>100</v>
+      </c>
+      <c r="G27">
+        <v>2674.19</v>
+      </c>
+      <c r="H27" s="6">
+        <v>324.39</v>
+      </c>
+      <c r="I27" s="6">
+        <v>362.67500000000001</v>
+      </c>
+      <c r="J27" s="23">
+        <f t="shared" si="0"/>
+        <v>687.06500000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="1">
+        <v>75</v>
+      </c>
+      <c r="G28">
+        <v>2606.83</v>
+      </c>
+      <c r="H28" s="6">
+        <v>705.303</v>
+      </c>
+      <c r="I28" s="6">
+        <v>1259.3</v>
+      </c>
+      <c r="J28" s="23">
+        <f t="shared" si="0"/>
+        <v>1964.6030000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="1">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>2505.92</v>
+      </c>
+      <c r="H29" s="6">
+        <v>742.76</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1988.75</v>
+      </c>
+      <c r="J29" s="23">
+        <f t="shared" si="0"/>
+        <v>2731.51</v>
+      </c>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="1">
+        <v>25</v>
+      </c>
+      <c r="G30">
+        <v>2456.61</v>
+      </c>
+      <c r="H30" s="6">
+        <v>790.20500000000004</v>
+      </c>
+      <c r="I30" s="6">
+        <v>2268.25</v>
+      </c>
+      <c r="J30" s="23">
+        <f t="shared" si="0"/>
+        <v>3058.4549999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>2755</v>
+      </c>
+      <c r="H31" s="6">
+        <v>777.33</v>
+      </c>
+      <c r="I31" s="6">
+        <v>2374.62</v>
+      </c>
+      <c r="J31" s="23">
+        <f t="shared" si="0"/>
+        <v>3151.95</v>
       </c>
     </row>
   </sheetData>
@@ -1231,17 +1351,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -1687,17 +1807,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -1963,17 +2083,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -2417,17 +2537,17 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
@@ -2887,17 +3007,17 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -3104,10 +3224,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,17 +3262,17 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -3224,7 +3344,7 @@
         <v>53.125999999999998</v>
       </c>
       <c r="I7" s="16">
-        <f t="shared" ref="I7:I25" si="0">G7+H7</f>
+        <f t="shared" ref="I7:I30" si="0">G7+H7</f>
         <v>301.26099999999997</v>
       </c>
       <c r="K7" s="11">
@@ -3661,6 +3781,111 @@
       </c>
       <c r="K25" s="11">
         <v>525.43091800000002</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="7">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>1373.87</v>
+      </c>
+      <c r="G26" s="6">
+        <v>168.40199999999999</v>
+      </c>
+      <c r="H26" s="6">
+        <v>266.73899999999998</v>
+      </c>
+      <c r="I26" s="23">
+        <f t="shared" si="0"/>
+        <v>435.14099999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="1">
+        <v>75</v>
+      </c>
+      <c r="F27">
+        <v>1459.23</v>
+      </c>
+      <c r="G27" s="6">
+        <v>532.85900000000004</v>
+      </c>
+      <c r="H27" s="6">
+        <v>96.248999999999995</v>
+      </c>
+      <c r="I27" s="23">
+        <f t="shared" si="0"/>
+        <v>629.10800000000006</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="1">
+        <v>50</v>
+      </c>
+      <c r="F28">
+        <v>1345.02</v>
+      </c>
+      <c r="G28" s="6">
+        <v>730.05</v>
+      </c>
+      <c r="H28" s="6">
+        <v>263.88</v>
+      </c>
+      <c r="I28" s="23">
+        <f t="shared" si="0"/>
+        <v>993.93</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="1">
+        <v>25</v>
+      </c>
+      <c r="F29">
+        <v>1280.42</v>
+      </c>
+      <c r="G29" s="6">
+        <v>796.47</v>
+      </c>
+      <c r="H29" s="6">
+        <v>255.392</v>
+      </c>
+      <c r="I29" s="23">
+        <f t="shared" si="0"/>
+        <v>1051.8620000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1173.3399999999999</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1006.97</v>
+      </c>
+      <c r="H30" s="6">
+        <v>253.054</v>
+      </c>
+      <c r="I30" s="23">
+        <f t="shared" si="0"/>
+        <v>1260.0240000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3676,7 +3901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -3714,17 +3939,17 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -3771,7 +3996,7 @@
       <c r="H6">
         <v>270.96600000000001</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="20">
         <f>G6+H6</f>
         <v>542.64400000000001</v>
       </c>
@@ -3795,7 +4020,7 @@
       <c r="H7">
         <v>558.84100000000001</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="20">
         <f t="shared" ref="I7:I25" si="0">G7+H7</f>
         <v>1431.4960000000001</v>
       </c>
@@ -3819,7 +4044,7 @@
       <c r="H8">
         <v>585.06700000000001</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="20">
         <f t="shared" si="0"/>
         <v>1637.2570000000001</v>
       </c>
@@ -3843,7 +4068,7 @@
       <c r="H9">
         <v>592.27700000000004</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="20">
         <f t="shared" si="0"/>
         <v>1760.4470000000001</v>
       </c>
@@ -3867,7 +4092,7 @@
       <c r="H10">
         <v>598.25199999999995</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="20">
         <f t="shared" si="0"/>
         <v>1889.252</v>
       </c>
@@ -3891,7 +4116,7 @@
       <c r="H11">
         <v>656.33600000000001</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="20">
         <f t="shared" si="0"/>
         <v>942.72</v>
       </c>
@@ -4011,7 +4236,7 @@
       <c r="H16">
         <v>666.274</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="20">
         <f t="shared" si="0"/>
         <v>970.279</v>
       </c>
@@ -4131,7 +4356,7 @@
       <c r="H21">
         <v>866.28</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="20">
         <f t="shared" si="0"/>
         <v>1290.77</v>
       </c>

</xml_diff>